<commit_message>
Re-executed Ledger and View Register page
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Ledger.data.xlsx
+++ b/tests/artifact/data/UI-Ledger.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="216">
   <si>
     <t>login.screen</t>
   </si>
@@ -160,7 +160,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:fb6542416f0f8d75513db5fd223b48100aefb8829d208c2a</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -436,7 +436,7 @@
     <t>account.selectField</t>
   </si>
   <si>
-    <t>//div/fieldset/div/div/div/input[@placeholder='select account']</t>
+    <t>//div[@class='card-body']/fieldset/div/div/div/input[@placeholder='select account']</t>
   </si>
   <si>
     <t>enter.accountValue</t>
@@ -575,19 +575,127 @@
   </si>
   <si>
     <t>//*[@class='popover-body']/div[3]/label/span</t>
+  </si>
+  <si>
+    <t>la.table.row.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr</t>
+  </si>
+  <si>
+    <t>la.date</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[1]/div</t>
+  </si>
+  <si>
+    <t>la.voucherNo</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[2]/div</t>
+  </si>
+  <si>
+    <t>la.status</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[3]/div</t>
+  </si>
+  <si>
+    <t>la.type</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[4]/div</t>
+  </si>
+  <si>
+    <t>la.particular</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[5]/div</t>
+  </si>
+  <si>
+    <t>la.debit</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[6]/div</t>
+  </si>
+  <si>
+    <t>la.credit</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[7]/div</t>
+  </si>
+  <si>
+    <t>la.balance</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[8]/div</t>
+  </si>
+  <si>
+    <t>la.date.values</t>
+  </si>
+  <si>
+    <t>/td[1]</t>
+  </si>
+  <si>
+    <t>la.voucherNo.values</t>
+  </si>
+  <si>
+    <t>/td[2]</t>
+  </si>
+  <si>
+    <t>la.status.values</t>
+  </si>
+  <si>
+    <t>/td[3]</t>
+  </si>
+  <si>
+    <t>la.type.values</t>
+  </si>
+  <si>
+    <t>/td[4]</t>
+  </si>
+  <si>
+    <t>la.particular.values</t>
+  </si>
+  <si>
+    <t>/td[5]</t>
+  </si>
+  <si>
+    <t>la.debit.values</t>
+  </si>
+  <si>
+    <t>/td[6]</t>
+  </si>
+  <si>
+    <t>la.credit.values</t>
+  </si>
+  <si>
+    <t>/td[7]</t>
+  </si>
+  <si>
+    <t>la.balance.values</t>
+  </si>
+  <si>
+    <t>/td[8]</t>
+  </si>
+  <si>
+    <t>ledger.showbutton</t>
+  </si>
+  <si>
+    <t>//div[@class='card-body']/fieldset/div/div/div/div/button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -632,14 +740,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -654,22 +768,62 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -680,14 +834,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -707,10 +853,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -721,57 +867,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -781,6 +880,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -791,187 +904,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,6 +1114,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1011,6 +1157,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,45 +1202,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1088,166 +1210,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1278,55 +1391,59 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1689,10 +1806,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2450,137 +2567,317 @@
         <v>179</v>
       </c>
     </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="12" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="21" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="20" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="19" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A25,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="27" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="37" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A26,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="28" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="38" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="29" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="39" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="30" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="40" stopIfTrue="1">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="41" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="32">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="42">
       <formula>LEN(TRIM(B26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="3" priority="21" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="31" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A27,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="22" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="32" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="33" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="24" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="5" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="35" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="36">
       <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="beginsWith" dxfId="3" priority="15" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="25" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A28,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="16" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="29" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="30">
       <formula>LEN(TRIM(B28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A94))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A94,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A94,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A94,LEN("//"))="//"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="beginsWith" dxfId="3" priority="5" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A95,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A95,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A95,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A95))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="33" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="43" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="34" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="36" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="46" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="48">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E63 B29:B39 B41:B63 B64:E1048576">
-    <cfRule type="expression" dxfId="5" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B20:B21">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="10">
+      <formula>LEN(TRIM(B20))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E63 B29:B39 B41:B63 B64:E1048576">
+    <cfRule type="expression" dxfId="5" priority="53" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="56">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="39" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A4:A24 A29:A93 A96:A1048576">
+    <cfRule type="beginsWith" dxfId="3" priority="49" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="40" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="52" stopIfTrue="1">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
re-executed the Ledger module
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Ledger.data.xlsx
+++ b/tests/artifact/data/UI-Ledger.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -30,12 +30,25 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
   <si>
     <t>login.screen</t>
   </si>
@@ -185,6 +198,18 @@
   </si>
   <si>
     <t>(//button[text()=' Open '])[79]</t>
+  </si>
+  <si>
+    <t>Org.locator</t>
+  </si>
+  <si>
+    <t>//tr/td[text()=' ']/parent::tr/td[@aria-colindex="4"]/button</t>
+  </si>
+  <si>
+    <t>Org.Name</t>
+  </si>
+  <si>
+    <t>LedgerTesting</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -450,7 +475,7 @@
     <t>enter.accountValue</t>
   </si>
   <si>
-    <t>Accion Labs Book Store</t>
+    <t>Sri Krishna Fancy Store</t>
   </si>
   <si>
     <t>click.monthlyLedger</t>
@@ -591,102 +616,6 @@
     <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr</t>
   </si>
   <si>
-    <t>la.date</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[1]/div</t>
-  </si>
-  <si>
-    <t>la.voucherNo</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[2]/div</t>
-  </si>
-  <si>
-    <t>la.status</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[3]/div</t>
-  </si>
-  <si>
-    <t>la.type</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[4]/div</t>
-  </si>
-  <si>
-    <t>la.particular</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[5]/div</t>
-  </si>
-  <si>
-    <t>la.debit</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[6]/div</t>
-  </si>
-  <si>
-    <t>la.credit</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[7]/div</t>
-  </si>
-  <si>
-    <t>la.balance</t>
-  </si>
-  <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/table/thead/tr/th[8]/div</t>
-  </si>
-  <si>
-    <t>la.date.values</t>
-  </si>
-  <si>
-    <t>/td[1]</t>
-  </si>
-  <si>
-    <t>la.voucherNo.values</t>
-  </si>
-  <si>
-    <t>/td[2]</t>
-  </si>
-  <si>
-    <t>la.status.values</t>
-  </si>
-  <si>
-    <t>/td[3]</t>
-  </si>
-  <si>
-    <t>la.type.values</t>
-  </si>
-  <si>
-    <t>/td[4]</t>
-  </si>
-  <si>
-    <t>la.particular.values</t>
-  </si>
-  <si>
-    <t>/td[5]</t>
-  </si>
-  <si>
-    <t>la.debit.values</t>
-  </si>
-  <si>
-    <t>/td[6]</t>
-  </si>
-  <si>
-    <t>la.credit.values</t>
-  </si>
-  <si>
-    <t>/td[7]</t>
-  </si>
-  <si>
-    <t>la.balance.values</t>
-  </si>
-  <si>
-    <t>/td[8]</t>
-  </si>
-  <si>
     <t>ledger.showbutton</t>
   </si>
   <si>
@@ -703,17 +632,104 @@
   </si>
   <si>
     <t>//button/div[contains(text(),' ')]</t>
+  </si>
+  <si>
+    <t>Ledger.List.Heading</t>
+  </si>
+  <si>
+    <t>//*[@class='bg-dark mb-4']/h6</t>
+  </si>
+  <si>
+    <t>type.searchValue</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Search Ledger']</t>
+  </si>
+  <si>
+    <t>Search.Values.Ledger</t>
+  </si>
+  <si>
+    <t>rt3</t>
+  </si>
+  <si>
+    <t>present.search.values</t>
+  </si>
+  <si>
+    <t>//tbody[@role='rowgroup']/tr[1]/td[2]/a</t>
+  </si>
+  <si>
+    <t>empty.search</t>
+  </si>
+  <si>
+    <t>Ledger.table.row.xpath</t>
+  </si>
+  <si>
+    <t>//tbody[@role='rowgroup']/tr</t>
+  </si>
+  <si>
+    <t>ledger.voucher.No</t>
+  </si>
+  <si>
+    <t>/td[2]/a</t>
+  </si>
+  <si>
+    <t>filters.button</t>
+  </si>
+  <si>
+    <t>//button[@id='select']</t>
+  </si>
+  <si>
+    <t>filters.credit</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Credit Only')]</t>
+  </si>
+  <si>
+    <t>filters.Debit</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Debit Only')]</t>
+  </si>
+  <si>
+    <t>filters.table</t>
+  </si>
+  <si>
+    <t>//div[@class='popover-body']</t>
+  </si>
+  <si>
+    <t>voucher.no.credit</t>
+  </si>
+  <si>
+    <t>//a[contains(@href,'#/Workflow/Transactions-Voucher/1886')]</t>
+  </si>
+  <si>
+    <t>VN.receipt.page</t>
+  </si>
+  <si>
+    <t>//div[@class='text-md-right col-md-6 order-md-2 col-12 order-1']//tbody/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>voucher.no.debit</t>
+  </si>
+  <si>
+    <t>//a[contains(@href,'#/Workflow/Transactions')]</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1238,16 +1254,16 @@
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1470,13 +1486,27 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color theme="1"/>
+        <b val="0"/>
+        <i val="1"/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.349986266670736"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.249946592608417"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.599963377788629"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1496,25 +1526,25 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.249946592608417"/>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.599963377788629"/>
+          <bgColor theme="0" tint="-0.14996795556505"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b val="1"/>
         <i val="1"/>
         <strike val="0"/>
-        <color theme="0" tint="-0.349986266670736"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="2"/>
+          <bgColor theme="0" tint="-0.0499893185216834"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,20 +1559,6 @@
       <numFmt numFmtId="49" formatCode="@"/>
       <fill>
         <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="1"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.0499893185216834"/>
-        </patternFill>
       </fill>
     </dxf>
   </dxfs>
@@ -1826,10 +1842,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B99" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2277,23 +2293,23 @@
         <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" ht="23.1" customHeight="1" spans="1:2">
       <c r="A56" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" ht="23.1" customHeight="1" spans="1:2">
       <c r="A57" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" ht="23.1" customHeight="1" spans="1:2">
@@ -2304,60 +2320,60 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" ht="23.1" customHeight="1" spans="1:3">
+    <row r="59" ht="23.1" customHeight="1" spans="1:2">
       <c r="A59" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="60" ht="23.1" customHeight="1" spans="1:2">
       <c r="A60" s="4" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" ht="23.1" customHeight="1" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" ht="23.1" customHeight="1" spans="1:3">
       <c r="A61" s="4" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>87</v>
+        <v>120</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="62" ht="23.1" customHeight="1" spans="1:2">
       <c r="A62" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" ht="23.1" customHeight="1" spans="1:2">
       <c r="A63" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
-        <v>120</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A64" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="65" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A65" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>123</v>
@@ -2399,7 +2415,7 @@
       <c r="A70" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2415,7 +2431,7 @@
       <c r="A72" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2615,7 +2631,7 @@
       <c r="A97" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="8" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2667,253 +2683,266 @@
         <v>199</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B113" s="2" t="s">
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1" t="s">
         <v>219</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="22" stopIfTrue="1">
+    <cfRule type="beginsWith" dxfId="0" priority="25" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A25,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="21" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="20" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="19" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A25,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
+    <cfRule type="expression" dxfId="4" priority="29" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="30">
       <formula>LEN(TRIM(B25))&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="23" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="37" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A26,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="38" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="39" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="40" stopIfTrue="1">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="41" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="42">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="3" priority="31" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="32" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="33" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="34" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="5" priority="35" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="36">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="beginsWith" dxfId="3" priority="25" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="43" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A28,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="46" stopIfTrue="1">
       <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="5" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="48">
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A94))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A94,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A94,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A94,LEN("//"))="//"</formula>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="beginsWith" dxfId="0" priority="37" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A29,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="38" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A29,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="39" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A29,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="40" stopIfTrue="1">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="beginsWith" dxfId="3" priority="5" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A95,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A95,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A95,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A95))&gt;0</formula>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" dxfId="4" priority="41" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="42">
+      <formula>LEN(TRIM(B29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="beginsWith" dxfId="0" priority="31" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A30,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="33" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="34" stopIfTrue="1">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="expression" dxfId="4" priority="35" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="36">
+      <formula>LEN(TRIM(B30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A96,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A96,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A96,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(A96))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="43" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="0" priority="49" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="46" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="52" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A27">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A26,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="53" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="48">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="54">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B21">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="16">
       <formula>LEN(TRIM(B20))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E63 B29:B39 B41:B63 B64:E1048576">
-    <cfRule type="expression" dxfId="5" priority="53" stopIfTrue="1">
+  <conditionalFormatting sqref="B26:B27">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(B26))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="56">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E1048576 B102:B1048576 B31:B41 B43:B100">
+    <cfRule type="expression" dxfId="4" priority="59" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="62">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A93 A96:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="49" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A4:A24 A31:A95 A97:A1048576">
+    <cfRule type="beginsWith" dxfId="0" priority="55" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="1" priority="56" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="2" priority="57" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="52" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="58" stopIfTrue="1">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Ledger and Transfer note script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Ledger.data.xlsx
+++ b/tests/artifact/data/UI-Ledger.data.xlsx
@@ -173,7 +173,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:1f05adcd8c26c19b8129a6bfec9e9fe9f9b9deb961baa281</t>
+    <t>crypt:3c7f85b459df6b6e19d1fda0badd66d0c803ec502466f2f6</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -209,7 +209,7 @@
     <t>Org.Name</t>
   </si>
   <si>
-    <t>LedgerTesting</t>
+    <t>TestingProduct</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -475,7 +475,7 @@
     <t>enter.accountValue</t>
   </si>
   <si>
-    <t>Sri Krishna Fancy Store</t>
+    <t>Bank A/C</t>
   </si>
   <si>
     <t>click.monthlyLedger</t>
@@ -1844,8 +1844,8 @@
   <sheetPr/>
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>

</xml_diff>